<commit_message>
update models and add jupyter examples
</commit_message>
<xml_diff>
--- a/Examples/AHP Ratings Cars/carModel_Ratings_Results.xlsx
+++ b/Examples/AHP Ratings Cars/carModel_Ratings_Results.xlsx
@@ -1560,6 +1560,41 @@
         <color rgb="ff0b30b5"/>
       </dataBar>
     </cfRule>
+    <cfRule type="dataBar" priority="81">
+      <dataBar showValue="1">
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="ff0b30b5"/>
+      </dataBar>
+    </cfRule>
+    <cfRule type="dataBar" priority="81">
+      <dataBar showValue="1">
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="ff0b30b5"/>
+      </dataBar>
+    </cfRule>
+    <cfRule type="dataBar" priority="81">
+      <dataBar showValue="1">
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="ff0b30b5"/>
+      </dataBar>
+    </cfRule>
+    <cfRule type="dataBar" priority="81">
+      <dataBar showValue="1">
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="ff0b30b5"/>
+      </dataBar>
+    </cfRule>
+    <cfRule type="dataBar" priority="81">
+      <dataBar showValue="1">
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="ff0b30b5"/>
+      </dataBar>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H13:H15">
     <cfRule type="dataBar" priority="1">
@@ -1646,6 +1681,27 @@
         <color rgb="ff0b30b5"/>
       </dataBar>
     </cfRule>
+    <cfRule type="dataBar" priority="81">
+      <dataBar showValue="1">
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="ff0b30b5"/>
+      </dataBar>
+    </cfRule>
+    <cfRule type="dataBar" priority="81">
+      <dataBar showValue="1">
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="ff0b30b5"/>
+      </dataBar>
+    </cfRule>
+    <cfRule type="dataBar" priority="81">
+      <dataBar showValue="1">
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="ff0b30b5"/>
+      </dataBar>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J21:J25">
     <cfRule type="dataBar" priority="1">
@@ -1788,6 +1844,41 @@
         <color rgb="ff0b30b5"/>
       </dataBar>
     </cfRule>
+    <cfRule type="dataBar" priority="81">
+      <dataBar showValue="1">
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="ff0b30b5"/>
+      </dataBar>
+    </cfRule>
+    <cfRule type="dataBar" priority="81">
+      <dataBar showValue="1">
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="ff0b30b5"/>
+      </dataBar>
+    </cfRule>
+    <cfRule type="dataBar" priority="81">
+      <dataBar showValue="1">
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="ff0b30b5"/>
+      </dataBar>
+    </cfRule>
+    <cfRule type="dataBar" priority="81">
+      <dataBar showValue="1">
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="ff0b30b5"/>
+      </dataBar>
+    </cfRule>
+    <cfRule type="dataBar" priority="81">
+      <dataBar showValue="1">
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="ff0b30b5"/>
+      </dataBar>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I31:I34">
     <cfRule type="dataBar" priority="1">
@@ -1902,6 +1993,34 @@
         <color rgb="ff0b30b5"/>
       </dataBar>
     </cfRule>
+    <cfRule type="dataBar" priority="81">
+      <dataBar showValue="1">
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="ff0b30b5"/>
+      </dataBar>
+    </cfRule>
+    <cfRule type="dataBar" priority="81">
+      <dataBar showValue="1">
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="ff0b30b5"/>
+      </dataBar>
+    </cfRule>
+    <cfRule type="dataBar" priority="81">
+      <dataBar showValue="1">
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="ff0b30b5"/>
+      </dataBar>
+    </cfRule>
+    <cfRule type="dataBar" priority="81">
+      <dataBar showValue="1">
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="ff0b30b5"/>
+      </dataBar>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H40:H42">
     <cfRule type="dataBar" priority="1">
@@ -1982,6 +2101,27 @@
       </dataBar>
     </cfRule>
     <cfRule type="dataBar" priority="61">
+      <dataBar showValue="1">
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="ff0b30b5"/>
+      </dataBar>
+    </cfRule>
+    <cfRule type="dataBar" priority="81">
+      <dataBar showValue="1">
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="ff0b30b5"/>
+      </dataBar>
+    </cfRule>
+    <cfRule type="dataBar" priority="81">
+      <dataBar showValue="1">
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="ff0b30b5"/>
+      </dataBar>
+    </cfRule>
+    <cfRule type="dataBar" priority="81">
       <dataBar showValue="1">
         <cfvo type="min" val="0"/>
         <cfvo type="max" val="0"/>
@@ -2515,7 +2655,97 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="120">
+  <dataValidations count="150">
+    <dataValidation sqref="B2" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A3:A7</formula1>
+    </dataValidation>
+    <dataValidation sqref="B3" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A3:A7</formula1>
+    </dataValidation>
+    <dataValidation sqref="B4" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A3:A7</formula1>
+    </dataValidation>
+    <dataValidation sqref="B5" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A3:A7</formula1>
+    </dataValidation>
+    <dataValidation sqref="B6" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A3:A7</formula1>
+    </dataValidation>
+    <dataValidation sqref="B7" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A3:A7</formula1>
+    </dataValidation>
+    <dataValidation sqref="C2" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A13:A15</formula1>
+    </dataValidation>
+    <dataValidation sqref="C3" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A13:A15</formula1>
+    </dataValidation>
+    <dataValidation sqref="C4" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A13:A15</formula1>
+    </dataValidation>
+    <dataValidation sqref="C5" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A13:A15</formula1>
+    </dataValidation>
+    <dataValidation sqref="C6" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A13:A15</formula1>
+    </dataValidation>
+    <dataValidation sqref="C7" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A13:A15</formula1>
+    </dataValidation>
+    <dataValidation sqref="D2" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A21:A25</formula1>
+    </dataValidation>
+    <dataValidation sqref="D3" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A21:A25</formula1>
+    </dataValidation>
+    <dataValidation sqref="D4" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A21:A25</formula1>
+    </dataValidation>
+    <dataValidation sqref="D5" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A21:A25</formula1>
+    </dataValidation>
+    <dataValidation sqref="D6" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A21:A25</formula1>
+    </dataValidation>
+    <dataValidation sqref="D7" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A21:A25</formula1>
+    </dataValidation>
+    <dataValidation sqref="E2" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A31:A34</formula1>
+    </dataValidation>
+    <dataValidation sqref="E3" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A31:A34</formula1>
+    </dataValidation>
+    <dataValidation sqref="E4" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A31:A34</formula1>
+    </dataValidation>
+    <dataValidation sqref="E5" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A31:A34</formula1>
+    </dataValidation>
+    <dataValidation sqref="E6" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A31:A34</formula1>
+    </dataValidation>
+    <dataValidation sqref="E7" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A31:A34</formula1>
+    </dataValidation>
+    <dataValidation sqref="F2" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A40:A42</formula1>
+    </dataValidation>
+    <dataValidation sqref="F3" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A40:A42</formula1>
+    </dataValidation>
+    <dataValidation sqref="F4" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A40:A42</formula1>
+    </dataValidation>
+    <dataValidation sqref="F5" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A40:A42</formula1>
+    </dataValidation>
+    <dataValidation sqref="F6" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A40:A42</formula1>
+    </dataValidation>
+    <dataValidation sqref="F7" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>=rating_scales!A40:A42</formula1>
+    </dataValidation>
     <dataValidation sqref="B2" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
       <formula1>=rating_scales!A3:A7</formula1>
     </dataValidation>

</xml_diff>